<commit_message>
add ini wlvl to modelsplitter and test
</commit_message>
<xml_diff>
--- a/tests/data/model_test/02_schematisation/model_settings.xlsx
+++ b/tests/data/model_test/02_schematisation/model_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\corp.hhnk.nl\data\Hydrologen_data\Data\02.modellen\model_test_v2\02_Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\corp.hhnk.nl\data\hydrologen_data\Data\github\wvangerwen\hhnk-threedi-tools\tests\data\model_test\02_schematisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E6081F-6F47-41F8-841F-02ECF7C8753F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F6EA5F-322E-473B-AA22-976182CA1981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1B3E74DF-8504-4A9A-9382-ED86C57E9482}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1B3E74DF-8504-4A9A-9382-ED86C57E9482}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>id</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>model_test_v2__1d2d_bgs</t>
+  </si>
+  <si>
+    <t>initial_waterlevel_file</t>
+  </si>
+  <si>
+    <t>rasters/initial_wlvl_2d_hoekje.tif</t>
   </si>
 </sst>
 </file>
@@ -203,12 +209,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -525,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E170822C-96C0-450A-813D-B7BC97529365}">
-  <dimension ref="A1:AS7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -537,7 +546,7 @@
     <col min="3" max="3" width="21.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="33.75" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" ht="33.75" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,64 +569,40 @@
         <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
-      <c r="AN1" s="1"/>
-      <c r="AO1" s="1"/>
-      <c r="AP1" s="1"/>
-      <c r="AQ1" s="1"/>
-      <c r="AR1" s="1"/>
-      <c r="AS1" s="1"/>
     </row>
-    <row r="2" spans="1:45" ht="33.75" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" ht="33.75" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -634,54 +619,28 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="1">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1">
         <v>900</v>
       </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
       <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
         <v>3</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1">
-        <v>1</v>
-      </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="2"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
-      <c r="AN2" s="1"/>
-      <c r="AO2" s="1"/>
-      <c r="AP2" s="1"/>
-      <c r="AQ2" s="1"/>
-      <c r="AR2" s="1"/>
-      <c r="AS2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:45" ht="33.75" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" ht="33.75" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -699,56 +658,30 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="I3" s="1">
+      <c r="H3" s="3"/>
+      <c r="J3" s="1">
         <v>300</v>
       </c>
-      <c r="J3" s="1">
-        <v>1</v>
-      </c>
       <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
         <v>3</v>
       </c>
-      <c r="L3" s="1">
-        <v>1</v>
-      </c>
       <c r="M3" s="1">
         <v>1</v>
       </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1">
-        <v>0</v>
-      </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="2"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
-      <c r="AN3" s="1"/>
-      <c r="AO3" s="1"/>
-      <c r="AP3" s="1"/>
-      <c r="AQ3" s="1"/>
-      <c r="AR3" s="1"/>
-      <c r="AS3" s="1"/>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:45" ht="45" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" ht="45" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -771,20 +704,20 @@
         <v>29</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>300</v>
       </c>
-      <c r="J4" s="1">
-        <v>1</v>
-      </c>
       <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
         <v>3</v>
       </c>
-      <c r="L4" s="1">
-        <v>1</v>
-      </c>
       <c r="M4" s="1">
         <v>1</v>
       </c>
@@ -792,7 +725,7 @@
         <v>1</v>
       </c>
       <c r="O4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="1">
         <v>0</v>
@@ -800,34 +733,11 @@
       <c r="Q4" s="1">
         <v>0</v>
       </c>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
-      <c r="AJ4" s="1"/>
-      <c r="AK4" s="1"/>
-      <c r="AL4" s="1"/>
-      <c r="AM4" s="1"/>
-      <c r="AN4" s="1"/>
-      <c r="AO4" s="1"/>
-      <c r="AP4" s="1"/>
-      <c r="AQ4" s="1"/>
-      <c r="AR4" s="1"/>
-      <c r="AS4" s="1"/>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:45" ht="45" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" ht="45" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -850,63 +760,40 @@
         <v>28</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>300</v>
       </c>
-      <c r="J5" s="1">
-        <v>1</v>
-      </c>
       <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1">
         <v>3</v>
       </c>
-      <c r="L5" s="1">
-        <v>1</v>
-      </c>
       <c r="M5" s="1">
         <v>1</v>
       </c>
       <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
         <v>2</v>
       </c>
-      <c r="O5" s="1">
-        <v>0</v>
-      </c>
       <c r="P5" s="1">
         <v>0</v>
       </c>
       <c r="Q5" s="1">
         <v>0</v>
       </c>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1"/>
-      <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="1"/>
-      <c r="AJ5" s="1"/>
-      <c r="AK5" s="1"/>
-      <c r="AL5" s="1"/>
-      <c r="AM5" s="1"/>
-      <c r="AN5" s="1"/>
-      <c r="AO5" s="1"/>
-      <c r="AP5" s="1"/>
-      <c r="AQ5" s="1"/>
-      <c r="AR5" s="1"/>
-      <c r="AS5" s="1"/>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:45" ht="45" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" ht="45" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -929,63 +816,40 @@
         <v>27</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>300</v>
       </c>
-      <c r="J6" s="1">
-        <v>1</v>
-      </c>
       <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
         <v>3</v>
       </c>
-      <c r="L6" s="1">
-        <v>1</v>
-      </c>
       <c r="M6" s="1">
         <v>1</v>
       </c>
       <c r="N6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1">
         <v>3</v>
       </c>
-      <c r="O6" s="1">
-        <v>0</v>
-      </c>
       <c r="P6" s="1">
         <v>0</v>
       </c>
       <c r="Q6" s="1">
         <v>0</v>
       </c>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
-      <c r="AK6" s="1"/>
-      <c r="AL6" s="1"/>
-      <c r="AM6" s="1"/>
-      <c r="AN6" s="1"/>
-      <c r="AO6" s="1"/>
-      <c r="AP6" s="1"/>
-      <c r="AQ6" s="1"/>
-      <c r="AR6" s="1"/>
-      <c r="AS6" s="1"/>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:45" ht="45" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" ht="45" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1008,61 +872,38 @@
         <v>31</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>300</v>
       </c>
-      <c r="J7" s="1">
-        <v>1</v>
-      </c>
       <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
         <v>3</v>
       </c>
-      <c r="L7" s="1">
-        <v>1</v>
-      </c>
       <c r="M7" s="1">
         <v>1</v>
       </c>
       <c r="N7" s="1">
+        <v>1</v>
+      </c>
+      <c r="O7" s="1">
         <v>4</v>
       </c>
-      <c r="O7" s="1">
-        <v>0</v>
-      </c>
       <c r="P7" s="1">
         <v>0</v>
       </c>
       <c r="Q7" s="1">
         <v>0</v>
       </c>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
-      <c r="AD7" s="1"/>
-      <c r="AE7" s="1"/>
-      <c r="AF7" s="1"/>
-      <c r="AG7" s="1"/>
-      <c r="AH7" s="1"/>
-      <c r="AI7" s="1"/>
-      <c r="AJ7" s="1"/>
-      <c r="AK7" s="1"/>
-      <c r="AL7" s="1"/>
-      <c r="AM7" s="1"/>
-      <c r="AN7" s="1"/>
-      <c r="AO7" s="1"/>
-      <c r="AP7" s="1"/>
-      <c r="AQ7" s="1"/>
-      <c r="AR7" s="1"/>
-      <c r="AS7" s="1"/>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
read ini wlvl agg type from sqlite
was default "max", will now be default "min", make sure we save that somewhere. added to issue #45
</commit_message>
<xml_diff>
--- a/tests/data/model_test/02_schematisation/model_settings.xlsx
+++ b/tests/data/model_test/02_schematisation/model_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\corp.hhnk.nl\data\hydrologen_data\Data\github\wvangerwen\hhnk-threedi-tools\tests\data\model_test\02_schematisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F6EA5F-322E-473B-AA22-976182CA1981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CCABCF-46C3-4923-B54D-709E2DE53AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1B3E74DF-8504-4A9A-9382-ED86C57E9482}"/>
+    <workbookView xWindow="3750" yWindow="6435" windowWidth="42510" windowHeight="17565" xr2:uid="{1B3E74DF-8504-4A9A-9382-ED86C57E9482}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>id</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>rasters/initial_wlvl_2d_hoekje.tif</t>
+  </si>
+  <si>
+    <t>water_level_ini_type</t>
   </si>
 </sst>
 </file>
@@ -534,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E170822C-96C0-450A-813D-B7BC97529365}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -546,7 +549,7 @@
     <col min="3" max="3" width="21.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="33.75" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" ht="33.75" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -572,37 +575,40 @@
         <v>40</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="33.75" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" ht="33.75" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -620,27 +626,28 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="1">
+      <c r="J2" s="1"/>
+      <c r="K2" s="1">
         <v>900</v>
       </c>
-      <c r="K2" s="1">
-        <v>0</v>
-      </c>
       <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
         <v>3</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="2"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1"/>
+      <c r="S2" s="2"/>
     </row>
-    <row r="3" spans="1:18" ht="33.75" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" ht="33.75" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -659,29 +666,30 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="3"/>
-      <c r="J3" s="1">
+      <c r="I3" s="3"/>
+      <c r="K3" s="1">
         <v>300</v>
       </c>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
       <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
         <v>3</v>
       </c>
-      <c r="M3" s="1">
-        <v>1</v>
-      </c>
       <c r="N3" s="1">
         <v>1</v>
       </c>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="2"/>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1"/>
+      <c r="S3" s="2"/>
     </row>
-    <row r="4" spans="1:18" ht="45" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:19" ht="45" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -706,21 +714,21 @@
       <c r="H4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>300</v>
       </c>
-      <c r="K4" s="1">
-        <v>1</v>
-      </c>
       <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
         <v>3</v>
       </c>
-      <c r="M4" s="1">
-        <v>1</v>
-      </c>
       <c r="N4" s="1">
         <v>1</v>
       </c>
@@ -728,7 +736,7 @@
         <v>1</v>
       </c>
       <c r="P4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="1">
         <v>0</v>
@@ -736,8 +744,11 @@
       <c r="R4" s="1">
         <v>0</v>
       </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" ht="45" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" ht="45" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -762,38 +773,41 @@
       <c r="H5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>300</v>
       </c>
-      <c r="K5" s="1">
-        <v>1</v>
-      </c>
       <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1">
         <v>3</v>
       </c>
-      <c r="M5" s="1">
-        <v>1</v>
-      </c>
       <c r="N5" s="1">
         <v>1</v>
       </c>
       <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1">
         <v>2</v>
       </c>
-      <c r="P5" s="1">
-        <v>0</v>
-      </c>
       <c r="Q5" s="1">
         <v>0</v>
       </c>
       <c r="R5" s="1">
         <v>0</v>
       </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" ht="45" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:19" ht="45" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -818,38 +832,41 @@
       <c r="H6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>300</v>
       </c>
-      <c r="K6" s="1">
-        <v>1</v>
-      </c>
       <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
         <v>3</v>
       </c>
-      <c r="M6" s="1">
-        <v>1</v>
-      </c>
       <c r="N6" s="1">
         <v>1</v>
       </c>
       <c r="O6" s="1">
+        <v>1</v>
+      </c>
+      <c r="P6" s="1">
         <v>3</v>
       </c>
-      <c r="P6" s="1">
-        <v>0</v>
-      </c>
       <c r="Q6" s="1">
         <v>0</v>
       </c>
       <c r="R6" s="1">
         <v>0</v>
       </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" ht="45" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19" ht="45" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -874,34 +891,37 @@
       <c r="H7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>300</v>
       </c>
-      <c r="K7" s="1">
-        <v>1</v>
-      </c>
       <c r="L7" s="1">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1">
         <v>3</v>
       </c>
-      <c r="M7" s="1">
-        <v>1</v>
-      </c>
       <c r="N7" s="1">
         <v>1</v>
       </c>
       <c r="O7" s="1">
+        <v>1</v>
+      </c>
+      <c r="P7" s="1">
         <v>4</v>
       </c>
-      <c r="P7" s="1">
-        <v>0</v>
-      </c>
       <c r="Q7" s="1">
         <v>0</v>
       </c>
       <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 2d wlvl to sim (#51)
* add raster to simulation

* test api calls

* add 2d wlvl to simulation gui

* add ini wlvl to modelsplitter and test

* batch calc option to enable lizard/aggregation

* add docstrings simdata

* Update README.md

* Update README.md

* fix data bug en batch neemt iwlvl goed mee

* read ini wlvl agg type from sqlite

was default "max", will now be default "min", make sure we save that somewhere. added to issue #45

* remove unused imports

---------

Co-authored-by: wietsevangerwen <41104904+wietsevangerwen@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tests/data/model_test/02_schematisation/model_settings.xlsx
+++ b/tests/data/model_test/02_schematisation/model_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\corp.hhnk.nl\data\Hydrologen_data\Data\02.modellen\model_test_v2\02_Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\corp.hhnk.nl\data\hydrologen_data\Data\github\wvangerwen\hhnk-threedi-tools\tests\data\model_test\02_schematisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E6081F-6F47-41F8-841F-02ECF7C8753F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CCABCF-46C3-4923-B54D-709E2DE53AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1B3E74DF-8504-4A9A-9382-ED86C57E9482}"/>
+    <workbookView xWindow="3750" yWindow="6435" windowWidth="42510" windowHeight="17565" xr2:uid="{1B3E74DF-8504-4A9A-9382-ED86C57E9482}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>id</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>model_test_v2__1d2d_bgs</t>
+  </si>
+  <si>
+    <t>initial_waterlevel_file</t>
+  </si>
+  <si>
+    <t>rasters/initial_wlvl_2d_hoekje.tif</t>
+  </si>
+  <si>
+    <t>water_level_ini_type</t>
   </si>
 </sst>
 </file>
@@ -203,12 +212,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -525,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E170822C-96C0-450A-813D-B7BC97529365}">
-  <dimension ref="A1:AS7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -537,7 +549,7 @@
     <col min="3" max="3" width="21.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="33.75" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" ht="33.75" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,64 +572,43 @@
         <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
-      <c r="AN1" s="1"/>
-      <c r="AO1" s="1"/>
-      <c r="AP1" s="1"/>
-      <c r="AQ1" s="1"/>
-      <c r="AR1" s="1"/>
-      <c r="AS1" s="1"/>
     </row>
-    <row r="2" spans="1:45" ht="33.75" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" ht="33.75" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -634,54 +625,29 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="1">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1">
         <v>900</v>
       </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
         <v>3</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1">
-        <v>0</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2" s="1"/>
-      <c r="Q2" s="2"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
-      <c r="AN2" s="1"/>
-      <c r="AO2" s="1"/>
-      <c r="AP2" s="1"/>
-      <c r="AQ2" s="1"/>
-      <c r="AR2" s="1"/>
-      <c r="AS2" s="1"/>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1"/>
+      <c r="S2" s="2"/>
     </row>
-    <row r="3" spans="1:45" ht="33.75" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" ht="33.75" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -699,56 +665,31 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="I3" s="1">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="K3" s="1">
         <v>300</v>
       </c>
-      <c r="J3" s="1">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
         <v>3</v>
       </c>
-      <c r="L3" s="1">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1"/>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
       <c r="O3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" s="1"/>
-      <c r="Q3" s="2"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
-      <c r="AN3" s="1"/>
-      <c r="AO3" s="1"/>
-      <c r="AP3" s="1"/>
-      <c r="AQ3" s="1"/>
-      <c r="AR3" s="1"/>
-      <c r="AS3" s="1"/>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1"/>
+      <c r="S3" s="2"/>
     </row>
-    <row r="4" spans="1:45" ht="45" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:19" ht="45" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -771,63 +712,43 @@
         <v>29</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="1">
+      <c r="K4" s="1">
         <v>300</v>
       </c>
-      <c r="J4" s="1">
-        <v>1</v>
-      </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
         <v>3</v>
       </c>
-      <c r="L4" s="1">
-        <v>1</v>
-      </c>
-      <c r="M4" s="1">
-        <v>1</v>
-      </c>
       <c r="N4" s="1">
         <v>1</v>
       </c>
       <c r="O4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="1">
         <v>0</v>
       </c>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
-      <c r="AJ4" s="1"/>
-      <c r="AK4" s="1"/>
-      <c r="AL4" s="1"/>
-      <c r="AM4" s="1"/>
-      <c r="AN4" s="1"/>
-      <c r="AO4" s="1"/>
-      <c r="AP4" s="1"/>
-      <c r="AQ4" s="1"/>
-      <c r="AR4" s="1"/>
-      <c r="AS4" s="1"/>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:45" ht="45" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" ht="45" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -850,63 +771,43 @@
         <v>28</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="1">
+      <c r="K5" s="1">
         <v>300</v>
       </c>
-      <c r="J5" s="1">
-        <v>1</v>
-      </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1">
         <v>3</v>
       </c>
-      <c r="L5" s="1">
-        <v>1</v>
-      </c>
-      <c r="M5" s="1">
-        <v>1</v>
-      </c>
       <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1">
         <v>2</v>
       </c>
-      <c r="O5" s="1">
-        <v>0</v>
-      </c>
-      <c r="P5" s="1">
-        <v>0</v>
-      </c>
       <c r="Q5" s="1">
         <v>0</v>
       </c>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1"/>
-      <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="1"/>
-      <c r="AJ5" s="1"/>
-      <c r="AK5" s="1"/>
-      <c r="AL5" s="1"/>
-      <c r="AM5" s="1"/>
-      <c r="AN5" s="1"/>
-      <c r="AO5" s="1"/>
-      <c r="AP5" s="1"/>
-      <c r="AQ5" s="1"/>
-      <c r="AR5" s="1"/>
-      <c r="AS5" s="1"/>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:45" ht="45" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:19" ht="45" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -929,63 +830,43 @@
         <v>27</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="1">
+      <c r="K6" s="1">
         <v>300</v>
       </c>
-      <c r="J6" s="1">
-        <v>1</v>
-      </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
         <v>3</v>
       </c>
-      <c r="L6" s="1">
-        <v>1</v>
-      </c>
-      <c r="M6" s="1">
-        <v>1</v>
-      </c>
       <c r="N6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1">
+        <v>1</v>
+      </c>
+      <c r="P6" s="1">
         <v>3</v>
       </c>
-      <c r="O6" s="1">
-        <v>0</v>
-      </c>
-      <c r="P6" s="1">
-        <v>0</v>
-      </c>
       <c r="Q6" s="1">
         <v>0</v>
       </c>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
-      <c r="AK6" s="1"/>
-      <c r="AL6" s="1"/>
-      <c r="AM6" s="1"/>
-      <c r="AN6" s="1"/>
-      <c r="AO6" s="1"/>
-      <c r="AP6" s="1"/>
-      <c r="AQ6" s="1"/>
-      <c r="AR6" s="1"/>
-      <c r="AS6" s="1"/>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:45" ht="45" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19" ht="45" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1008,61 +889,41 @@
         <v>31</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="1">
+      <c r="K7" s="1">
         <v>300</v>
       </c>
-      <c r="J7" s="1">
-        <v>1</v>
-      </c>
-      <c r="K7" s="1">
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1">
         <v>3</v>
       </c>
-      <c r="L7" s="1">
-        <v>1</v>
-      </c>
-      <c r="M7" s="1">
-        <v>1</v>
-      </c>
       <c r="N7" s="1">
+        <v>1</v>
+      </c>
+      <c r="O7" s="1">
+        <v>1</v>
+      </c>
+      <c r="P7" s="1">
         <v>4</v>
       </c>
-      <c r="O7" s="1">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1">
-        <v>0</v>
-      </c>
       <c r="Q7" s="1">
         <v>0</v>
       </c>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
-      <c r="AD7" s="1"/>
-      <c r="AE7" s="1"/>
-      <c r="AF7" s="1"/>
-      <c r="AG7" s="1"/>
-      <c r="AH7" s="1"/>
-      <c r="AI7" s="1"/>
-      <c r="AJ7" s="1"/>
-      <c r="AK7" s="1"/>
-      <c r="AL7" s="1"/>
-      <c r="AM7" s="1"/>
-      <c r="AN7" s="1"/>
-      <c r="AO7" s="1"/>
-      <c r="AP7" s="1"/>
-      <c r="AQ7" s="1"/>
-      <c r="AR7" s="1"/>
-      <c r="AS7" s="1"/>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>